<commit_message>
pattern matching to seperate dataframes working but does not enforce number and character lengths
</commit_message>
<xml_diff>
--- a/Sample_Sheet_Test.xlsx
+++ b/Sample_Sheet_Test.xlsx
@@ -1,24 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chase.schwalbach/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="525" windowWidth="28800" windowHeight="16380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="170720_K00342_0050_AHKKNLBBXX.S" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="80">
   <si>
     <t>[Header]</t>
   </si>
@@ -261,6 +253,12 @@
   </si>
   <si>
     <t>CS</t>
+  </si>
+  <si>
+    <t>175RES1030_3T</t>
+  </si>
+  <si>
+    <t>176RES940_3T</t>
   </si>
 </sst>
 </file>
@@ -303,8 +301,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -568,7 +594,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -578,18 +604,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="3" width="24.25" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="16.75" customWidth="1"/>
+    <col min="6" max="6" width="17.75" customWidth="1"/>
+    <col min="8" max="8" width="25.75" customWidth="1"/>
+    <col min="9" max="9" width="46.75" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -597,7 +632,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -605,7 +640,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -613,7 +648,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -621,7 +656,7 @@
         <v>42936</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -629,7 +664,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -637,7 +672,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -645,7 +680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -653,7 +688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -661,27 +696,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -689,7 +724,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -697,12 +732,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -731,12 +766,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="F22" t="s">
         <v>24</v>
@@ -745,7 +780,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -759,7 +794,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -773,7 +808,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -787,7 +822,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -801,7 +836,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2</v>
       </c>
@@ -815,7 +850,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2</v>
       </c>
@@ -829,7 +864,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2</v>
       </c>
@@ -843,7 +878,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2</v>
       </c>
@@ -857,7 +892,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
@@ -871,7 +906,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>3</v>
       </c>
@@ -885,7 +920,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3</v>
       </c>
@@ -899,7 +934,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3</v>
       </c>
@@ -913,7 +948,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3</v>
       </c>
@@ -927,7 +962,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>3</v>
       </c>
@@ -941,7 +976,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>3</v>
       </c>
@@ -955,7 +990,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>4</v>
       </c>
@@ -969,7 +1004,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>4</v>
       </c>
@@ -983,12 +1018,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F40" t="s">
         <v>28</v>
@@ -997,7 +1032,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>4</v>
       </c>
@@ -1011,7 +1046,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>4</v>
       </c>
@@ -1025,7 +1060,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>5</v>
       </c>
@@ -1039,7 +1074,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>5</v>
       </c>
@@ -1053,7 +1088,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>5</v>
       </c>
@@ -1067,7 +1102,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>5</v>
       </c>
@@ -1081,7 +1116,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>5</v>
       </c>
@@ -1095,7 +1130,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>6</v>
       </c>
@@ -1109,7 +1144,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>6</v>
       </c>
@@ -1123,7 +1158,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>6</v>
       </c>
@@ -1137,7 +1172,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>6</v>
       </c>
@@ -1151,7 +1186,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>6</v>
       </c>
@@ -1165,7 +1200,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>7</v>
       </c>
@@ -1179,7 +1214,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>7</v>
       </c>
@@ -1193,7 +1228,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>7</v>
       </c>
@@ -1207,7 +1242,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>7</v>
       </c>
@@ -1221,7 +1256,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>7</v>
       </c>
@@ -1235,7 +1270,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>7</v>
       </c>
@@ -1249,7 +1284,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>8</v>
       </c>
@@ -1263,7 +1298,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>8</v>
       </c>
@@ -1277,7 +1312,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>8</v>
       </c>
@@ -1291,7 +1326,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>8</v>
       </c>
@@ -1305,7 +1340,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
reverting xlsx to original doc recieved in zip. (had made changes in testing)
Signed-off-by: Steve Dolatowski <sdolatowski@chartertsp.com>
</commit_message>
<xml_diff>
--- a/Sample_Sheet_Test.xlsx
+++ b/Sample_Sheet_Test.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chase.schwalbach/Desktop/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="525" windowWidth="28800" windowHeight="16380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="170720_K00342_0050_AHKKNLBBXX.S" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="78">
   <si>
     <t>[Header]</t>
   </si>
@@ -253,12 +261,6 @@
   </si>
   <si>
     <t>CS</t>
-  </si>
-  <si>
-    <t>175RES1030_3T</t>
-  </si>
-  <si>
-    <t>176RES940_3T</t>
   </si>
 </sst>
 </file>
@@ -301,36 +303,8 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7D7D7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
-    </tableStyle>
-  </tableStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -594,7 +568,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -604,27 +578,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="3" width="24.25" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
-    <col min="5" max="5" width="16.75" customWidth="1"/>
-    <col min="6" max="6" width="17.75" customWidth="1"/>
-    <col min="8" max="8" width="25.75" customWidth="1"/>
-    <col min="9" max="9" width="46.75" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -632,7 +597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -640,7 +605,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -648,7 +613,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -656,7 +621,7 @@
         <v>42936</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -664,7 +629,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -672,7 +637,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -680,7 +645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -688,7 +653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -696,27 +661,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -724,7 +689,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -732,12 +697,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -766,12 +731,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="F22" t="s">
         <v>24</v>
@@ -780,7 +745,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -794,7 +759,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -808,7 +773,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1</v>
       </c>
@@ -822,7 +787,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -836,7 +801,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2</v>
       </c>
@@ -850,7 +815,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2</v>
       </c>
@@ -864,7 +829,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2</v>
       </c>
@@ -878,7 +843,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2</v>
       </c>
@@ -892,7 +857,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2</v>
       </c>
@@ -906,7 +871,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3</v>
       </c>
@@ -920,7 +885,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3</v>
       </c>
@@ -934,7 +899,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3</v>
       </c>
@@ -948,7 +913,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3</v>
       </c>
@@ -962,7 +927,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3</v>
       </c>
@@ -976,7 +941,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>3</v>
       </c>
@@ -990,7 +955,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>4</v>
       </c>
@@ -1004,7 +969,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>4</v>
       </c>
@@ -1018,12 +983,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="F40" t="s">
         <v>28</v>
@@ -1032,7 +997,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>4</v>
       </c>
@@ -1046,7 +1011,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>4</v>
       </c>
@@ -1060,7 +1025,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>5</v>
       </c>
@@ -1074,7 +1039,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>5</v>
       </c>
@@ -1088,7 +1053,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>5</v>
       </c>
@@ -1102,7 +1067,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>5</v>
       </c>
@@ -1116,7 +1081,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>5</v>
       </c>
@@ -1130,7 +1095,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>6</v>
       </c>
@@ -1144,7 +1109,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>6</v>
       </c>
@@ -1158,7 +1123,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>6</v>
       </c>
@@ -1172,7 +1137,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>6</v>
       </c>
@@ -1186,7 +1151,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>6</v>
       </c>
@@ -1200,7 +1165,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>7</v>
       </c>
@@ -1214,7 +1179,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>7</v>
       </c>
@@ -1228,7 +1193,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>7</v>
       </c>
@@ -1242,7 +1207,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>7</v>
       </c>
@@ -1256,7 +1221,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>7</v>
       </c>
@@ -1270,7 +1235,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>7</v>
       </c>
@@ -1284,7 +1249,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>8</v>
       </c>
@@ -1298,7 +1263,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>8</v>
       </c>
@@ -1312,7 +1277,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>8</v>
       </c>
@@ -1326,7 +1291,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>8</v>
       </c>
@@ -1340,7 +1305,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>8</v>
       </c>

</xml_diff>